<commit_message>
bug fixes, added recipies
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cs6al\Desktop\satisfactory-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEEB85C-4121-44FA-8387-19B87BB7A764}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62B2097-45D5-469E-968F-1FC8C225E5D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C3F026C2-FBB1-49F3-9423-EEFA2A2B539D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="119">
   <si>
     <t>Building</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Stator</t>
   </si>
   <si>
-    <t>Morot</t>
-  </si>
-  <si>
     <t>Fabric</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
   </si>
   <si>
     <t>Mycelia</t>
-  </si>
-  <si>
-    <t>Qurtz Crystal</t>
   </si>
   <si>
     <t xml:space="preserve">Miner </t>
@@ -770,17 +764,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD20FF2-F9E1-4355-8BC2-F438D78DA23F}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
@@ -847,10 +841,10 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1">
         <v>480</v>
@@ -865,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -957,7 +951,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -982,7 +976,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
@@ -1005,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1">
         <v>480</v>
@@ -1022,28 +1016,22 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>480</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1051,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1066,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1077,13 +1065,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
@@ -1092,56 +1080,50 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
       </c>
       <c r="E13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H13" s="1">
-        <v>3</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="b">
         <v>0</v>
@@ -1150,21 +1132,27 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
         <v>8</v>
@@ -1176,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="1">
         <v>4</v>
@@ -1184,42 +1172,42 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="1">
         <v>4</v>
-      </c>
-      <c r="E16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="b">
         <v>0</v>
@@ -1228,10 +1216,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1239,10 +1227,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <v>4</v>
@@ -1254,10 +1242,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1265,7 +1253,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1280,10 +1268,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1291,10 +1279,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
@@ -1306,10 +1294,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="H20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1317,10 +1305,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
@@ -1332,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1343,25 +1331,25 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
       </c>
       <c r="E22" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1369,13 +1357,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E23" s="1" t="b">
         <v>0</v>
@@ -1384,10 +1372,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H23" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1395,25 +1383,25 @@
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
       </c>
       <c r="E24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H24" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1421,13 +1409,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" s="1" t="b">
         <v>0</v>
@@ -1436,10 +1424,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H25" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1447,10 +1435,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
@@ -1462,10 +1450,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1473,10 +1461,10 @@
         <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
@@ -1488,24 +1476,24 @@
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E28" s="1" t="b">
         <v>0</v>
@@ -1514,30 +1502,24 @@
         <v>0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H28" s="1">
-        <v>4</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E29" s="1" t="b">
         <v>0</v>
@@ -1546,16 +1528,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H29" s="1">
-        <v>3</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J29" s="1">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1563,13 +1539,13 @@
         <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E30" s="1" t="b">
         <v>0</v>
@@ -1578,16 +1554,16 @@
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="H30" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J30" s="1">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1595,13 +1571,13 @@
         <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1" t="b">
         <v>0</v>
@@ -1610,16 +1586,16 @@
         <v>0</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H31" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J31" s="1">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1627,13 +1603,13 @@
         <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1" t="b">
         <v>0</v>
@@ -1642,16 +1618,16 @@
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="H32" s="1">
         <v>3</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J32" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -1659,13 +1635,13 @@
         <v>45</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E33" s="1" t="b">
         <v>0</v>
@@ -1674,16 +1650,16 @@
         <v>0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="H33" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="J33" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -1691,31 +1667,31 @@
         <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="J34" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -1723,10 +1699,10 @@
         <v>45</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
         <v>12</v>
@@ -1738,16 +1714,16 @@
         <v>0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="H35" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J35" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -1755,31 +1731,31 @@
         <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E36" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H36" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="J36" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -1787,45 +1763,45 @@
         <v>45</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E37" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="H37" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="J37" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="1">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E38" s="1" t="b">
         <v>0</v>
@@ -1834,86 +1810,62 @@
         <v>0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H38" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J38" s="1">
-        <v>15</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L38" s="1">
-        <v>5</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N38" s="1">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E39" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H39" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="J39" s="1">
-        <v>12</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L39" s="1">
-        <v>18</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N39" s="1">
-        <v>90</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
       <c r="D40" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>0</v>
@@ -1922,43 +1874,31 @@
         <v>0</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H40" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J40" s="1">
         <v>2</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L40" s="1">
-        <v>3</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N40" s="1">
-        <v>21</v>
-      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="1">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1">
         <v>60</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1">
-        <v>24</v>
-      </c>
       <c r="E41" s="1" t="b">
         <v>0</v>
       </c>
@@ -1966,36 +1906,30 @@
         <v>0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="H41" s="1">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J41" s="1">
-        <v>10</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L41" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E42" s="1" t="b">
         <v>0</v>
@@ -2004,30 +1938,36 @@
         <v>0</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H42" s="1">
         <v>5</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="J42" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L42" s="1">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N42" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
@@ -2042,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="H43" s="1">
         <v>10</v>
@@ -2051,27 +1991,33 @@
         <v>20</v>
       </c>
       <c r="J43" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="L43" s="1">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N43" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="1">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E44" s="1" t="b">
         <v>0</v>
@@ -2080,36 +2026,42 @@
         <v>0</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H44" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="J44" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L44" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N44" s="1">
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E45" s="1" t="b">
         <v>0</v>
@@ -2118,144 +2070,180 @@
         <v>0</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H45" s="1">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J45" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="L45" s="1">
-        <v>15</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N45" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E46" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>83</v>
+      <c r="F46" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H46" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="J46" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L46" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E47" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>84</v>
+      <c r="F47" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="H47" s="1">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="1">
+        <v>14</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L47" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C48" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E48" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>99</v>
+      <c r="F48" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="H48" s="1">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J48" s="1">
+        <v>5</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L48" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C49" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D49" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E49" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>101</v>
+      <c r="F49" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J49" s="1">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="1">
+        <v>15</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N49" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -2263,39 +2251,39 @@
         <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C50" s="1">
         <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E50" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H50" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="J50" s="1">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C51" s="1">
         <v>12</v>
@@ -2307,18 +2295,12 @@
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H51" s="1">
-        <v>1</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J51" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2339,51 +2321,45 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C53" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D53" s="1">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E53" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H53" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J53" s="1">
-        <v>4</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L53" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -2391,31 +2367,31 @@
         <v>45</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="C54" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D54" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E54" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="H54" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="J54" s="1">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -2423,42 +2399,42 @@
         <v>45</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="C55" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D55" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E55" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="H55" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="J55" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C56" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D56" s="1">
         <v>8</v>
@@ -2467,95 +2443,83 @@
         <v>0</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H56" s="1">
         <v>1</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J56" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C57" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D57" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E57" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H57" s="1">
-        <v>18</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J57" s="1">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L57" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C58" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E58" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="H58" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="J58" s="1">
-        <v>10</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L58" s="1">
-        <v>36</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N58" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -2563,304 +2527,316 @@
         <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C59" s="1">
         <v>3</v>
       </c>
       <c r="D59" s="1">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E59" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>91</v>
+      <c r="F59" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H59" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="J59" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="C60" s="1">
         <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="H60" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="J60" s="1">
-        <v>2</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L60" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C61" s="1">
         <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E61" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="H61" s="1">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J61" s="1">
         <v>10</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L61" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C62" s="1">
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E62" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H62" s="1">
+        <v>8</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J62" s="1">
+        <v>10</v>
+      </c>
+      <c r="K62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H62" s="1">
-        <v>6</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J62" s="1">
-        <v>20</v>
+      <c r="L62" s="1">
+        <v>36</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N62" s="1">
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C63" s="1">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E63" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H63" s="1">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C64" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E64" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="H64" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="J64" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="1">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1">
+        <v>40</v>
+      </c>
+      <c r="E65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H65" s="1">
+        <v>10</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J65" s="1">
+        <v>10</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="1">
-        <v>3</v>
-      </c>
-      <c r="D65" s="1">
+      <c r="B66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="1">
+        <v>3</v>
+      </c>
+      <c r="D66" s="1">
         <v>20</v>
       </c>
-      <c r="E65" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="E66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H65" s="1">
-        <v>3</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J65" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="1">
-        <v>6</v>
-      </c>
-      <c r="D66" s="1">
-        <v>8</v>
-      </c>
-      <c r="E66" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H66" s="1">
         <v>6</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="J66" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C67" s="1">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D67" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E67" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H67" s="1">
-        <v>3</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J67" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C68" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D68" s="1">
         <v>8</v>
@@ -2869,383 +2845,359 @@
         <v>0</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H68" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="J68" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" s="1">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1">
         <v>20</v>
       </c>
-      <c r="C69" s="1">
+      <c r="E69" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" s="1">
+        <v>3</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J69" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" s="1">
+        <v>6</v>
+      </c>
+      <c r="D70" s="1">
         <v>8</v>
       </c>
-      <c r="D69" s="1">
-        <v>12</v>
-      </c>
-      <c r="E69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H69" s="1">
-        <v>4</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J69" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C70" s="1">
-        <v>24</v>
-      </c>
-      <c r="D70" s="1">
+      <c r="E70" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H70" s="1">
         <v>6</v>
       </c>
-      <c r="E70" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H70" s="1">
-        <v>16</v>
-      </c>
       <c r="I70" s="1" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="J70" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C71" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D71" s="1">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H71" s="1">
+        <v>3</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J71" s="1">
         <v>6</v>
       </c>
-      <c r="E71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H71" s="1">
-        <v>12</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J71" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C72" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D72" s="1">
+        <v>8</v>
+      </c>
+      <c r="E72" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H72" s="1">
+        <v>3</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J72" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="1">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1">
+        <v>12</v>
+      </c>
+      <c r="E73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H73" s="1">
+        <v>4</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J73" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C74" s="1">
         <v>24</v>
       </c>
-      <c r="E72" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H72" s="1">
-        <v>4</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J72" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C73" s="1">
-        <v>3</v>
-      </c>
-      <c r="D73" s="1">
-        <v>64</v>
-      </c>
-      <c r="E73" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H73" s="1">
-        <v>20</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J73" s="1">
-        <v>80</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L73" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C74" s="1">
-        <v>3</v>
-      </c>
       <c r="D74" s="1">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="E74" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="H74" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="J74" s="1">
         <v>24</v>
       </c>
-      <c r="K74" s="1" t="s">
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="1">
+        <v>24</v>
+      </c>
+      <c r="D75" s="1">
+        <v>6</v>
+      </c>
+      <c r="E75" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L74" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C75" s="1">
-        <v>3</v>
-      </c>
-      <c r="D75" s="1">
-        <v>48</v>
-      </c>
-      <c r="E75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G75" s="1" t="s">
+      <c r="H75" s="1">
+        <v>12</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H75" s="1">
-        <v>66</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="J75" s="1">
-        <v>48</v>
-      </c>
-      <c r="K75" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L75" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C76" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D76" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E76" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H76" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="J76" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C77" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D77" s="1">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E77" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="H77" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="J77" s="1">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="L77" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C78" s="1">
         <v>3</v>
       </c>
       <c r="D78" s="1">
-        <v>300</v>
+        <v>64</v>
       </c>
       <c r="E78" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="H78" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="J78" s="1">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="L78" s="1">
-        <v>3</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N78" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C79" s="1">
         <v>3</v>
@@ -3257,112 +3209,258 @@
         <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="H79" s="1">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="J79" s="1">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="L79" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C80" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D80" s="1">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E80" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H80" s="1">
         <v>8</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="J80" s="1">
-        <v>4</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L80" s="1">
-        <v>8</v>
-      </c>
-      <c r="M80" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N80" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C81" s="1">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D81" s="1">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="E81" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>110</v>
+      <c r="F81" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H81" s="1">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>74</v>
       </c>
       <c r="J81" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1">
+        <v>300</v>
+      </c>
+      <c r="E82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H82" s="1">
+        <v>25</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J82" s="1">
+        <v>10</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L82" s="1">
+        <v>3</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N82" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C83" s="1">
+        <v>3</v>
+      </c>
+      <c r="D83" s="1">
+        <v>48</v>
+      </c>
+      <c r="E83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H83" s="1">
+        <v>10</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J83" s="1">
+        <v>1</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L83" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" s="1">
+        <v>3</v>
+      </c>
+      <c r="D84" s="1">
+        <v>64</v>
+      </c>
+      <c r="E84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H84" s="1">
+        <v>8</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J84" s="1">
+        <v>4</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L84" s="1">
+        <v>8</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N84" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C85" s="1">
+        <v>35</v>
+      </c>
+      <c r="D85" s="1">
+        <v>120</v>
+      </c>
+      <c r="E85" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H85" s="1">
         <v>45</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="I85" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J85" s="1">
+        <v>45</v>
+      </c>
+      <c r="K85" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L81" s="1">
+      <c r="L85" s="1">
         <v>45</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="M85" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N81" s="1">
+      <c r="N85" s="1">
         <v>60</v>
       </c>
     </row>

</xml_diff>